<commit_message>
Update Automation TestCase & Update Excel Data
</commit_message>
<xml_diff>
--- a/src/main/resources/OLMS_TestData.xlsx
+++ b/src/main/resources/OLMS_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hthuy\Documents\intelliJ Project\Nhom B - Testing 01 - Cybersoft\OLMS_Test-Selenium\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0401C445-3820-44C5-AA0F-276656A709DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8B3A9D-6559-4614-9E8D-93FC9FFB0663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -359,149 +359,335 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="30">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -547,160 +733,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -709,6 +741,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -716,80 +757,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -809,35 +776,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9957896B-AFDF-4710-86A5-06155D1B9C7B}" name="Table5" displayName="Table5" ref="A1:B2" totalsRowShown="0" headerRowBorderDxfId="30" tableBorderDxfId="31" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9957896B-AFDF-4710-86A5-06155D1B9C7B}" name="Table5" displayName="Table5" ref="A1:B2" totalsRowShown="0" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
   <autoFilter ref="A1:B2" xr:uid="{9957896B-AFDF-4710-86A5-06155D1B9C7B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{648B7877-530B-44D0-A524-BB5FDD729E28}" name="username" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{E4C6462B-CA12-4F96-881E-05EDC94A3D45}" name="password" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{648B7877-530B-44D0-A524-BB5FDD729E28}" name="username" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E4C6462B-CA12-4F96-881E-05EDC94A3D45}" name="password" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EAB0CC52-9F69-401E-B99E-A7C5C878F539}" name="Table4" displayName="Table4" ref="A1:O9" totalsRowShown="0" headerRowBorderDxfId="24" tableBorderDxfId="25" totalsRowBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EAB0CC52-9F69-401E-B99E-A7C5C878F539}" name="Table4" displayName="Table4" ref="A1:O9" totalsRowShown="0" dataDxfId="5" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
   <autoFilter ref="A1:O9" xr:uid="{EAB0CC52-9F69-401E-B99E-A7C5C878F539}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{653FB087-36D6-4FB1-A7FB-73F605917649}" name="tenLopHoc" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{BBFBE4EE-1C77-4168-936B-14EDF37ED967}" name="doTuoi" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{71E26DCD-A5F2-4DB3-AF0E-C32B96F2D3AA}" name="ngayBatDau" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{02FF3287-47D8-48B5-B4EF-4E309F8816AB}" name="khoaHoc" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{8BDE880E-93D0-44DE-A02D-40393168E649}" name="lichHoc" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{A289B1C0-DEE0-4C7D-B5B7-A48FAF864810}" name="phongHoc" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{D76DF92B-968E-46B1-BF25-3F47E72288CE}" name="thoiGianDungLop" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{65E19D13-CF36-4FB6-9BB2-36478BB7DB52}" name="giaoVienVN" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{27D094E7-A692-4CDD-86F7-5FB98540EF8E}" name="giaoVienNuocNgoai" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{C5EC160C-FCA5-4733-BA9D-AB6D35AE1761}" name="troGiang" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{291740A6-EEB1-4585-9CE0-5499A5D20E4D}" name="nguoiNhanXet" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{0439A81E-5C6C-48F0-ABE4-9B7EFD749199}" name="trangThai" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{503A73A9-FE2D-49E9-9586-4335ACD9F1E7}" name="hocVien" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{C2DAF932-10BA-4A60-8F58-406909342C32}" name="soBuoi" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{8AF4BCB1-CDA1-4513-87C0-98A54E63309E}" name="ghiChu" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{653FB087-36D6-4FB1-A7FB-73F605917649}" name="tenLopHoc" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{BBFBE4EE-1C77-4168-936B-14EDF37ED967}" name="doTuoi" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{71E26DCD-A5F2-4DB3-AF0E-C32B96F2D3AA}" name="ngayBatDau" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{02FF3287-47D8-48B5-B4EF-4E309F8816AB}" name="khoaHoc" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{8BDE880E-93D0-44DE-A02D-40393168E649}" name="lichHoc" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{A289B1C0-DEE0-4C7D-B5B7-A48FAF864810}" name="phongHoc" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{D76DF92B-968E-46B1-BF25-3F47E72288CE}" name="thoiGianDungLop" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{65E19D13-CF36-4FB6-9BB2-36478BB7DB52}" name="giaoVienVN" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{27D094E7-A692-4CDD-86F7-5FB98540EF8E}" name="giaoVienNuocNgoai" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{C5EC160C-FCA5-4733-BA9D-AB6D35AE1761}" name="troGiang" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{291740A6-EEB1-4585-9CE0-5499A5D20E4D}" name="nguoiNhanXet" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{0439A81E-5C6C-48F0-ABE4-9B7EFD749199}" name="trangThai" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{503A73A9-FE2D-49E9-9586-4335ACD9F1E7}" name="hocVien" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{C2DAF932-10BA-4A60-8F58-406909342C32}" name="soBuoi" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{8AF4BCB1-CDA1-4513-87C0-98A54E63309E}" name="ghiChu" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1108,14 +1075,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -1126,25 +1093,25 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:Z2">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+  <conditionalFormatting sqref="A2:Z2 C3:Z10 A3:B9">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="9" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1160,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3B65CD-E13D-4637-B865-423827C201E4}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,307 +1166,307 @@
       <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="6">
         <f ca="1">TODAY()</f>
-        <v>45769</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>45784</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="N2" s="12">
+      <c r="N2" s="8">
         <v>0</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="6">
         <v>0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="6">
         <v>54871</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3" s="6">
         <v>10</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4" s="6">
         <v>-10</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6">
         <v>9999999999</v>
       </c>
-      <c r="O5" s="1"/>
+      <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="6">
         <v>999999999</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1" t="s">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="O6" s="1"/>
+      <c r="O6" s="6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="1">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6">
         <v>-100</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="6" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1" t="s">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="O7" s="1"/>
+      <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="6" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="3" t="s">
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="O8" s="1"/>
+      <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:Z9">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="13" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>